<commit_message>
Little changes andclean code
</commit_message>
<xml_diff>
--- a/files/Formulario Web.xlsx
+++ b/files/Formulario Web.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookair/Documents/9. Octubre_2023/9. Procesamiento cvs txt/9.2 Muestra Fuentes de Información Cierre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Todo\Documentos\Santiago\3_Trabajo Profesional\Full-Stack-Projects\Bodega\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA3E81D-AB5F-9941-A667-8459357B27A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F941080E-74CF-485B-98BE-405D910A706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="3" r:id="rId1"/>
@@ -23,11 +23,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Verificada!$A$1:$GH$1</definedName>
   </definedNames>
   <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="238">
   <si>
     <t>Código prestador</t>
   </si>
@@ -879,12 +890,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="BASE_CARACT"/>
       <sheetName val="copia base johanna - 18-10-2023"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1179,11 +1188,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93654267-6479-904D-893E-2C7D975AEF0D}">
   <dimension ref="A1:EU11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1649,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>22125</v>
       </c>
@@ -1648,8 +1659,8 @@
       <c r="C2">
         <v>2023</v>
       </c>
-      <c r="D2" t="s">
-        <v>151</v>
+      <c r="D2">
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>152</v>
@@ -2084,7 +2095,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14185</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14182</v>
       </c>
@@ -2970,7 +2981,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14182</v>
       </c>
@@ -3410,7 +3421,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>22115</v>
       </c>
@@ -3850,7 +3861,7 @@
         <v>3003433982</v>
       </c>
     </row>
-    <row r="7" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22133</v>
       </c>
@@ -4296,7 +4307,7 @@
         <v>3017109931</v>
       </c>
     </row>
-    <row r="8" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22166</v>
       </c>
@@ -4751,7 +4762,7 @@
         <v>3013332987</v>
       </c>
     </row>
-    <row r="9" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22133</v>
       </c>
@@ -5197,7 +5208,7 @@
         <v>3123733846</v>
       </c>
     </row>
-    <row r="10" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22103</v>
       </c>
@@ -5640,7 +5651,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22133</v>
       </c>
@@ -6095,101 +6106,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="45.33203125" customWidth="1"/>
-    <col min="7" max="7" width="59.1640625" customWidth="1"/>
-    <col min="8" max="8" width="32.83203125" customWidth="1"/>
-    <col min="11" max="11" width="54.6640625" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" customWidth="1"/>
-    <col min="13" max="15" width="41.83203125" customWidth="1"/>
-    <col min="16" max="16" width="6.1640625" customWidth="1"/>
-    <col min="17" max="19" width="41.83203125" customWidth="1"/>
-    <col min="20" max="20" width="6.1640625" customWidth="1"/>
-    <col min="21" max="23" width="41.83203125" customWidth="1"/>
-    <col min="24" max="24" width="6.1640625" customWidth="1"/>
-    <col min="25" max="27" width="41.83203125" customWidth="1"/>
-    <col min="28" max="28" width="6.1640625" customWidth="1"/>
-    <col min="29" max="31" width="41.83203125" customWidth="1"/>
-    <col min="32" max="32" width="6.1640625" customWidth="1"/>
-    <col min="33" max="35" width="41.83203125" customWidth="1"/>
-    <col min="36" max="36" width="6.1640625" customWidth="1"/>
-    <col min="37" max="39" width="41.83203125" customWidth="1"/>
-    <col min="40" max="40" width="6.1640625" customWidth="1"/>
-    <col min="41" max="43" width="41.83203125" customWidth="1"/>
-    <col min="44" max="44" width="6.1640625" customWidth="1"/>
-    <col min="45" max="47" width="41.83203125" customWidth="1"/>
-    <col min="48" max="48" width="6.1640625" customWidth="1"/>
-    <col min="49" max="51" width="41.83203125" customWidth="1"/>
-    <col min="52" max="52" width="6.1640625" customWidth="1"/>
-    <col min="53" max="55" width="41.83203125" customWidth="1"/>
-    <col min="56" max="56" width="6.1640625" customWidth="1"/>
-    <col min="57" max="59" width="41.83203125" customWidth="1"/>
-    <col min="60" max="60" width="6.1640625" customWidth="1"/>
-    <col min="61" max="61" width="33.1640625" customWidth="1"/>
-    <col min="62" max="63" width="41.83203125" customWidth="1"/>
-    <col min="64" max="64" width="6.1640625" customWidth="1"/>
-    <col min="65" max="67" width="41.83203125" customWidth="1"/>
-    <col min="68" max="68" width="6.1640625" customWidth="1"/>
-    <col min="69" max="71" width="41.83203125" customWidth="1"/>
-    <col min="72" max="72" width="6.1640625" customWidth="1"/>
-    <col min="73" max="75" width="41.83203125" customWidth="1"/>
-    <col min="76" max="76" width="6.1640625" customWidth="1"/>
-    <col min="77" max="79" width="41.83203125" customWidth="1"/>
-    <col min="80" max="80" width="6.1640625" customWidth="1"/>
-    <col min="81" max="84" width="41.83203125" customWidth="1"/>
-    <col min="85" max="85" width="6.1640625" customWidth="1"/>
-    <col min="86" max="88" width="54.1640625" customWidth="1"/>
-    <col min="89" max="89" width="6.1640625" customWidth="1"/>
-    <col min="90" max="92" width="54.1640625" customWidth="1"/>
-    <col min="93" max="93" width="6.1640625" customWidth="1"/>
-    <col min="94" max="96" width="54.1640625" customWidth="1"/>
-    <col min="97" max="97" width="6.1640625" customWidth="1"/>
-    <col min="98" max="100" width="54.1640625" customWidth="1"/>
-    <col min="101" max="101" width="6.1640625" customWidth="1"/>
-    <col min="102" max="104" width="54.1640625" customWidth="1"/>
-    <col min="105" max="105" width="6.1640625" customWidth="1"/>
-    <col min="106" max="108" width="54.1640625" customWidth="1"/>
-    <col min="109" max="109" width="6.1640625" customWidth="1"/>
-    <col min="110" max="112" width="54.1640625" customWidth="1"/>
-    <col min="113" max="113" width="6.1640625" customWidth="1"/>
-    <col min="114" max="116" width="54.1640625" customWidth="1"/>
-    <col min="117" max="117" width="6.1640625" customWidth="1"/>
-    <col min="118" max="120" width="54.1640625" customWidth="1"/>
-    <col min="121" max="121" width="6.1640625" customWidth="1"/>
-    <col min="122" max="124" width="54.1640625" customWidth="1"/>
-    <col min="125" max="125" width="6.1640625" customWidth="1"/>
-    <col min="126" max="128" width="54.1640625" customWidth="1"/>
-    <col min="129" max="129" width="6.1640625" customWidth="1"/>
-    <col min="130" max="132" width="54.1640625" customWidth="1"/>
-    <col min="133" max="133" width="6.1640625" customWidth="1"/>
-    <col min="134" max="134" width="54.1640625" customWidth="1"/>
-    <col min="135" max="135" width="6.1640625" customWidth="1"/>
-    <col min="136" max="141" width="54.1640625" customWidth="1"/>
-    <col min="142" max="142" width="6.1640625" customWidth="1"/>
-    <col min="143" max="143" width="54.1640625" customWidth="1"/>
-    <col min="144" max="144" width="46.83203125" customWidth="1"/>
-    <col min="145" max="145" width="46.1640625" customWidth="1"/>
-    <col min="146" max="146" width="49.33203125" customWidth="1"/>
-    <col min="147" max="148" width="54.1640625" customWidth="1"/>
-    <col min="149" max="149" width="6.1640625" customWidth="1"/>
-    <col min="150" max="150" width="54.1640625" customWidth="1"/>
-    <col min="151" max="151" width="6.1640625" customWidth="1"/>
-    <col min="152" max="157" width="54.1640625" customWidth="1"/>
-    <col min="158" max="158" width="6.1640625" customWidth="1"/>
-    <col min="159" max="164" width="54.1640625" customWidth="1"/>
-    <col min="165" max="165" width="6.1640625" customWidth="1"/>
-    <col min="166" max="168" width="64.33203125" customWidth="1"/>
-    <col min="169" max="169" width="41.83203125" customWidth="1"/>
+    <col min="1" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" customWidth="1"/>
+    <col min="7" max="7" width="59.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
+    <col min="11" max="11" width="54.7109375" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="15" width="41.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="17" max="19" width="41.85546875" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" customWidth="1"/>
+    <col min="21" max="23" width="41.85546875" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" customWidth="1"/>
+    <col min="25" max="27" width="41.85546875" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" customWidth="1"/>
+    <col min="29" max="31" width="41.85546875" customWidth="1"/>
+    <col min="32" max="32" width="6.140625" customWidth="1"/>
+    <col min="33" max="35" width="41.85546875" customWidth="1"/>
+    <col min="36" max="36" width="6.140625" customWidth="1"/>
+    <col min="37" max="39" width="41.85546875" customWidth="1"/>
+    <col min="40" max="40" width="6.140625" customWidth="1"/>
+    <col min="41" max="43" width="41.85546875" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
+    <col min="45" max="47" width="41.85546875" customWidth="1"/>
+    <col min="48" max="48" width="6.140625" customWidth="1"/>
+    <col min="49" max="51" width="41.85546875" customWidth="1"/>
+    <col min="52" max="52" width="6.140625" customWidth="1"/>
+    <col min="53" max="55" width="41.85546875" customWidth="1"/>
+    <col min="56" max="56" width="6.140625" customWidth="1"/>
+    <col min="57" max="59" width="41.85546875" customWidth="1"/>
+    <col min="60" max="60" width="6.140625" customWidth="1"/>
+    <col min="61" max="61" width="33.140625" customWidth="1"/>
+    <col min="62" max="63" width="41.85546875" customWidth="1"/>
+    <col min="64" max="64" width="6.140625" customWidth="1"/>
+    <col min="65" max="67" width="41.85546875" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" customWidth="1"/>
+    <col min="69" max="71" width="41.85546875" customWidth="1"/>
+    <col min="72" max="72" width="6.140625" customWidth="1"/>
+    <col min="73" max="75" width="41.85546875" customWidth="1"/>
+    <col min="76" max="76" width="6.140625" customWidth="1"/>
+    <col min="77" max="79" width="41.85546875" customWidth="1"/>
+    <col min="80" max="80" width="6.140625" customWidth="1"/>
+    <col min="81" max="84" width="41.85546875" customWidth="1"/>
+    <col min="85" max="85" width="6.140625" customWidth="1"/>
+    <col min="86" max="88" width="54.140625" customWidth="1"/>
+    <col min="89" max="89" width="6.140625" customWidth="1"/>
+    <col min="90" max="92" width="54.140625" customWidth="1"/>
+    <col min="93" max="93" width="6.140625" customWidth="1"/>
+    <col min="94" max="96" width="54.140625" customWidth="1"/>
+    <col min="97" max="97" width="6.140625" customWidth="1"/>
+    <col min="98" max="100" width="54.140625" customWidth="1"/>
+    <col min="101" max="101" width="6.140625" customWidth="1"/>
+    <col min="102" max="104" width="54.140625" customWidth="1"/>
+    <col min="105" max="105" width="6.140625" customWidth="1"/>
+    <col min="106" max="108" width="54.140625" customWidth="1"/>
+    <col min="109" max="109" width="6.140625" customWidth="1"/>
+    <col min="110" max="112" width="54.140625" customWidth="1"/>
+    <col min="113" max="113" width="6.140625" customWidth="1"/>
+    <col min="114" max="116" width="54.140625" customWidth="1"/>
+    <col min="117" max="117" width="6.140625" customWidth="1"/>
+    <col min="118" max="120" width="54.140625" customWidth="1"/>
+    <col min="121" max="121" width="6.140625" customWidth="1"/>
+    <col min="122" max="124" width="54.140625" customWidth="1"/>
+    <col min="125" max="125" width="6.140625" customWidth="1"/>
+    <col min="126" max="128" width="54.140625" customWidth="1"/>
+    <col min="129" max="129" width="6.140625" customWidth="1"/>
+    <col min="130" max="132" width="54.140625" customWidth="1"/>
+    <col min="133" max="133" width="6.140625" customWidth="1"/>
+    <col min="134" max="134" width="54.140625" customWidth="1"/>
+    <col min="135" max="135" width="6.140625" customWidth="1"/>
+    <col min="136" max="141" width="54.140625" customWidth="1"/>
+    <col min="142" max="142" width="6.140625" customWidth="1"/>
+    <col min="143" max="143" width="54.140625" customWidth="1"/>
+    <col min="144" max="144" width="46.85546875" customWidth="1"/>
+    <col min="145" max="145" width="46.140625" customWidth="1"/>
+    <col min="146" max="146" width="49.28515625" customWidth="1"/>
+    <col min="147" max="148" width="54.140625" customWidth="1"/>
+    <col min="149" max="149" width="6.140625" customWidth="1"/>
+    <col min="150" max="150" width="54.140625" customWidth="1"/>
+    <col min="151" max="151" width="6.140625" customWidth="1"/>
+    <col min="152" max="157" width="54.140625" customWidth="1"/>
+    <col min="158" max="158" width="6.140625" customWidth="1"/>
+    <col min="159" max="164" width="54.140625" customWidth="1"/>
+    <col min="165" max="165" width="6.140625" customWidth="1"/>
+    <col min="166" max="168" width="64.28515625" customWidth="1"/>
+    <col min="169" max="169" width="41.85546875" customWidth="1"/>
     <col min="179" max="190" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:190" s="1" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:190" s="1" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6759,7 +6770,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>22125</v>
       </c>
@@ -7362,7 +7373,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14185</v>
       </c>
@@ -7959,7 +7970,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14182</v>
       </c>
@@ -8559,7 +8570,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14182</v>
       </c>
@@ -9156,7 +9167,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>22115</v>
       </c>
@@ -9750,7 +9761,7 @@
         <v>3003433982</v>
       </c>
     </row>
-    <row r="7" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22133</v>
       </c>
@@ -10350,7 +10361,7 @@
         <v>3017109931</v>
       </c>
     </row>
-    <row r="8" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22166</v>
       </c>
@@ -10959,7 +10970,7 @@
         <v>3013332987</v>
       </c>
     </row>
-    <row r="9" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22133</v>
       </c>
@@ -11559,7 +11570,7 @@
         <v>3123733846</v>
       </c>
     </row>
-    <row r="10" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22103</v>
       </c>
@@ -12156,7 +12167,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22133</v>
       </c>
@@ -12756,7 +12767,7 @@
         <v>3005791599</v>
       </c>
     </row>
-    <row r="15" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>237</v>
       </c>
@@ -12767,7 +12778,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:190" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -12776,7 +12787,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -12785,7 +12796,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -12794,7 +12805,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>

</xml_diff>